<commit_message>
Added drop downs for data type and thousands separator.
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esriis-my.sharepoint.com/personal/lisa7570_esri_com/Documents/2022 Projects/Alias Updater on GItHub/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esriis-my.sharepoint.com/personal/mark9020_esri_com/Documents/Documents/Scripts/Python/AliasUpdater/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{3C71C269-F504-490D-B617-A6E79E9A85B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB188167-6AAD-40CB-BE0C-F3E115C84E95}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="8_{3C71C269-F504-490D-B617-A6E79E9A85B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59E40315-FB52-485D-99FB-E9665B6B6673}"/>
   <bookViews>
-    <workbookView xWindow="1725" yWindow="1875" windowWidth="28800" windowHeight="15435" xr2:uid="{799F5197-C316-4D4E-986D-D1C535813486}"/>
+    <workbookView xWindow="2985" yWindow="1770" windowWidth="21600" windowHeight="11385" xr2:uid="{799F5197-C316-4D4E-986D-D1C535813486}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Lookup" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="FieldType">Lookup!$A$2:$A$16</definedName>
+    <definedName name="Seperator">Lookup!$B$2:$B$3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>field</t>
   </si>
@@ -87,10 +92,52 @@
     <t>thousandsSeparator</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
+    <t>nameOrTitle</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>typeOrCategory</t>
+  </si>
+  <si>
+    <t>percentageOrRatio</t>
+  </si>
+  <si>
+    <t>measurement</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>emailAddress</t>
+  </si>
+  <si>
+    <t>orderedOrRanked</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>locationOrPlaceName</t>
+  </si>
+  <si>
+    <t>coordinate</t>
+  </si>
+  <si>
+    <t>Field Type</t>
+  </si>
+  <si>
+    <t>Seperator</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -145,10 +192,33 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5B88EB1E-F513-4663-BD0A-03CE5CFC1005}" name="Table1" displayName="Table1" ref="A1:A16" totalsRowShown="0">
+  <autoFilter ref="A1:A16" xr:uid="{5B88EB1E-F513-4663-BD0A-03CE5CFC1005}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A16">
+    <sortCondition ref="A2:A16"/>
+  </sortState>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{40574A58-0675-4F10-B4EC-27891FBC68A8}" name="Field Type"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{39863BEA-04A8-46E3-8749-0AFD943CA050}" name="Table2" displayName="Table2" ref="B1:B3" totalsRowShown="0">
+  <autoFilter ref="B1:B3" xr:uid="{39863BEA-04A8-46E3-8749-0AFD943CA050}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{E026A4A1-BB88-48DD-A0ED-40A960E36542}" name="Seperator"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -186,7 +256,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -292,7 +362,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -434,7 +504,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -444,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5D1F2C-B61D-4E30-87E4-5701F2FC541C}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,6 +560,9 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -505,7 +578,7 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -525,30 +598,135 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations xWindow="560" yWindow="486" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instructions" prompt="Select a data type from the list." sqref="D1:D1048576" xr:uid="{4E232263-D8A1-47F9-BC56-E00CD791D3C6}">
+      <formula1>FieldType</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instructions" prompt="Select a value from the list." sqref="F1:F1048576" xr:uid="{AC9CE8E7-9C25-4582-9551-9F4B59D5EC2C}">
+      <formula1>Seperator</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A9729BA-CAAA-4F2A-9821-B8F1AA17D9C1}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BD1A32E3DCB70F44965014DCA3718728" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6169f1c5c7e53f161b248dfa127f5433">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="df8e6348-0292-409e-8383-6cad4b57558a" xmlns:ns4="b7e3458c-8b2d-4d8f-bebd-ecb4f4eceda2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40f782e3d277ace46757ed729bd1f727" ns3:_="" ns4:_="">
     <xsd:import namespace="df8e6348-0292-409e-8383-6cad4b57558a"/>
@@ -771,32 +949,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07EF1C28-D541-459E-AF89-4878930C7E32}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b7e3458c-8b2d-4d8f-bebd-ecb4f4eceda2"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="df8e6348-0292-409e-8383-6cad4b57558a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA3FA5B7-0CCE-43CE-9944-8DF3257EAE18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE169458-A0BA-4083-9786-E5EDCDBA85C3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -813,4 +981,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA3FA5B7-0CCE-43CE-9944-8DF3257EAE18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07EF1C28-D541-459E-AF89-4878930C7E32}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b7e3458c-8b2d-4d8f-bebd-ecb4f4eceda2"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="df8e6348-0292-409e-8383-6cad4b57558a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>